<commit_message>
Added boost converter to fuel cell network to follow charge sustaining algorithm (R2020a and higher).
</commit_message>
<xml_diff>
--- a/Libraries/Vehicle/Power/FuelCell/sm_car_data_FuelCell_FuelCell1Motor.xlsx
+++ b/Libraries/Vehicle/Power/FuelCell/sm_car_data_FuelCell_FuelCell1Motor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Others\smiller\ssvt\Libraries\Vehicle\Power\FuelCell\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\smiller\simscape\demo\allsimscape\cars\vehicle-templates\zFuelCellConv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E931A2A8-9CCD-4F8F-B510-0DE78BE065C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097AAE50-D5FB-460A-999A-7393862FF377}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="10152" xr2:uid="{3EB3AC41-B7D3-4E4D-A710-77CB91E8EAF9}"/>
+    <workbookView xWindow="6912" yWindow="1524" windowWidth="15516" windowHeight="11316" xr2:uid="{3EB3AC41-B7D3-4E4D-A710-77CB91E8EAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="FuelCell_A1_default" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="166">
   <si>
     <t>Units</t>
   </si>
@@ -456,6 +456,81 @@
   </si>
   <si>
     <t>FuelCell_A1_default</t>
+  </si>
+  <si>
+    <t>ConverterB</t>
+  </si>
+  <si>
+    <t>rOn</t>
+  </si>
+  <si>
+    <t>Diode</t>
+  </si>
+  <si>
+    <t>vForward</t>
+  </si>
+  <si>
+    <t>1/Ohm</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Cext</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Cint</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TFiltI0</t>
+  </si>
+  <si>
+    <t>Bias</t>
+  </si>
+  <si>
+    <t>GOff</t>
+  </si>
+  <si>
+    <t>Lint</t>
+  </si>
+  <si>
+    <t>transferCoefficientB</t>
+  </si>
+  <si>
+    <t>Abstract DC-DC</t>
+  </si>
+  <si>
+    <t>Boost Converter</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -919,29 +994,29 @@
   <sheetPr>
     <tabColor rgb="FFCCFF66"/>
   </sheetPr>
-  <dimension ref="A1:K175"/>
+  <dimension ref="A1:K193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D171" activePane="bottomRight" state="frozen"/>
       <selection activeCell="E9" sqref="E9"/>
       <selection pane="topRight" activeCell="E9" sqref="E9"/>
       <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="H181" sqref="H181"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.109375" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
     <col min="6" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="10" max="15" width="6.6640625" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="15" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -961,7 +1036,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
@@ -975,7 +1050,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>6</v>
       </c>
@@ -989,7 +1064,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
@@ -1003,7 +1078,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>34</v>
       </c>
@@ -1023,7 +1098,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
@@ -1039,7 +1114,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
@@ -1055,7 +1130,7 @@
         <v>1.7670999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5" t="s">
@@ -1071,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
@@ -1087,7 +1162,7 @@
         <v>1.5E-5</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5" t="s">
@@ -1101,7 +1176,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5" t="s">
@@ -1116,7 +1191,7 @@
       </c>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
@@ -1130,7 +1205,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
@@ -1145,7 +1220,7 @@
       </c>
       <c r="I13" s="14"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5" t="s">
@@ -1160,7 +1235,7 @@
         <v>0.101325</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5" t="s">
@@ -1175,7 +1250,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5" t="s">
@@ -1190,7 +1265,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
@@ -1205,7 +1280,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
@@ -1220,7 +1295,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
@@ -1235,7 +1310,7 @@
         <v>4.0000000000000001E-8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
@@ -1250,7 +1325,7 @@
         <v>293.14999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5" t="s">
         <v>47</v>
@@ -1268,7 +1343,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5" t="s">
@@ -1284,7 +1359,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5" t="s">
@@ -1300,7 +1375,7 @@
         <v>1.7670999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="5"/>
       <c r="C24" s="5" t="s">
@@ -1316,7 +1391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
@@ -1332,7 +1407,7 @@
         <v>1.5E-5</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
@@ -1346,7 +1421,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
@@ -1360,7 +1435,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
@@ -1374,7 +1449,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
@@ -1388,7 +1463,7 @@
         <v>3.66</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
@@ -1403,7 +1478,7 @@
         <v>0.101325</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
@@ -1418,7 +1493,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="5" t="s">
         <v>20</v>
@@ -1435,7 +1510,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
@@ -1450,7 +1525,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5" t="s">
@@ -1465,7 +1540,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5" t="s">
@@ -1481,7 +1556,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="5" t="s">
         <v>17</v>
@@ -1498,7 +1573,7 @@
         <v>1.7670999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="5" t="s">
         <v>53</v>
@@ -1513,7 +1588,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5" t="s">
@@ -1526,7 +1601,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5" t="s">
@@ -1539,7 +1614,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5" t="s">
@@ -1552,7 +1627,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
@@ -1567,7 +1642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5" t="s">
@@ -1582,7 +1657,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="5" t="s">
         <v>11</v>
@@ -1599,7 +1674,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5" t="s">
@@ -1614,7 +1689,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5" t="s">
@@ -1632,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="8"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5" t="s">
@@ -1650,7 +1725,7 @@
         <v>1.7670999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="8"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5" t="s">
@@ -1665,7 +1740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="8"/>
       <c r="B48" s="5"/>
       <c r="C48" s="5" t="s">
@@ -1680,7 +1755,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="8"/>
       <c r="B49" s="5"/>
       <c r="C49" s="5" t="s">
@@ -1695,7 +1770,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>8</v>
       </c>
@@ -1712,7 +1787,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="5" t="s">
         <v>66</v>
@@ -1727,7 +1802,7 @@
         <v>45500</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="5" t="s">
         <v>68</v>
@@ -1742,7 +1817,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="5" t="s">
         <v>70</v>
@@ -1757,7 +1832,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="5" t="s">
         <v>72</v>
@@ -1770,7 +1845,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="5" t="s">
         <v>73</v>
@@ -1783,7 +1858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="5" t="s">
         <v>27</v>
@@ -1796,7 +1871,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="5" t="s">
         <v>74</v>
@@ -1809,7 +1884,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="5"/>
       <c r="B58" s="5" t="s">
         <v>29</v>
@@ -1822,7 +1897,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="5"/>
       <c r="B59" s="5" t="s">
         <v>77</v>
@@ -1835,7 +1910,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>79</v>
       </c>
@@ -1850,7 +1925,7 @@
         <v>0.101325</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="5" t="s">
         <v>41</v>
@@ -1863,7 +1938,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="5"/>
       <c r="B62" s="5" t="s">
         <v>80</v>
@@ -1883,7 +1958,7 @@
         <v>0.28077000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="5" t="s">
         <v>81</v>
@@ -1898,7 +1973,7 @@
         <v>3.1415999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>82</v>
       </c>
@@ -1915,7 +1990,7 @@
         <v>0.101325</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="5"/>
       <c r="B65" s="5" t="s">
         <v>41</v>
@@ -1930,7 +2005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="s">
         <v>80</v>
@@ -1952,7 +2027,7 @@
         <v>1.3849999999999999E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="5" t="s">
         <v>81</v>
@@ -1967,7 +2042,7 @@
         <v>3.1415999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>83</v>
       </c>
@@ -1984,7 +2059,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="5"/>
       <c r="B69" s="5" t="s">
         <v>49</v>
@@ -1999,7 +2074,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
       <c r="B70" s="5" t="s">
         <v>85</v>
@@ -2012,7 +2087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="5" t="s">
         <v>51</v>
@@ -2022,7 +2097,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="s">
         <v>81</v>
@@ -2035,7 +2110,7 @@
         <v>3.1415999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
       <c r="B73" s="5" t="s">
         <v>87</v>
@@ -2045,7 +2120,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>88</v>
       </c>
@@ -2060,7 +2135,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="5"/>
       <c r="B75" s="5" t="s">
         <v>40</v>
@@ -2075,7 +2150,7 @@
         <v>0.101325</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="s">
         <v>41</v>
@@ -2090,7 +2165,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="5" t="s">
         <v>80</v>
@@ -2109,7 +2184,7 @@
         <v>0.28077000000000002</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="5"/>
       <c r="B78" s="5" t="s">
         <v>89</v>
@@ -2122,7 +2197,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="5"/>
       <c r="B79" s="5" t="s">
         <v>91</v>
@@ -2141,7 +2216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="5"/>
       <c r="B80" s="5" t="s">
         <v>81</v>
@@ -2154,7 +2229,7 @@
         <v>3.1415999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>92</v>
       </c>
@@ -2169,7 +2244,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="5"/>
       <c r="B82" s="5" t="s">
         <v>40</v>
@@ -2184,7 +2259,7 @@
         <v>0.101325</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="5"/>
       <c r="B83" s="5" t="s">
         <v>41</v>
@@ -2199,7 +2274,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="5" t="s">
         <v>80</v>
@@ -2218,7 +2293,7 @@
         <v>1.3849999999999999E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="5"/>
       <c r="B85" s="5" t="s">
         <v>89</v>
@@ -2231,7 +2306,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="5"/>
       <c r="B86" s="5" t="s">
         <v>91</v>
@@ -2250,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="5"/>
       <c r="B87" s="5" t="s">
         <v>81</v>
@@ -2263,7 +2338,7 @@
         <v>3.1415999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>93</v>
       </c>
@@ -2278,7 +2353,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="5"/>
       <c r="B89" s="5" t="s">
         <v>49</v>
@@ -2291,7 +2366,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="5"/>
       <c r="B90" s="5" t="s">
         <v>85</v>
@@ -2304,7 +2379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="5" t="s">
         <v>51</v>
@@ -2314,7 +2389,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="5"/>
       <c r="B92" s="5" t="s">
         <v>81</v>
@@ -2327,7 +2402,7 @@
         <v>3.1415999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="5"/>
       <c r="B93" s="5" t="s">
         <v>87</v>
@@ -2337,7 +2412,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>94</v>
       </c>
@@ -2352,7 +2427,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="5"/>
       <c r="B95" s="5" t="s">
         <v>49</v>
@@ -2365,7 +2440,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="5"/>
       <c r="B96" s="5" t="s">
         <v>85</v>
@@ -2378,7 +2453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="5"/>
       <c r="B97" s="5" t="s">
         <v>51</v>
@@ -2388,7 +2463,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="5"/>
       <c r="B98" s="5" t="s">
         <v>81</v>
@@ -2401,7 +2476,7 @@
         <v>3.1415999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="5"/>
       <c r="B99" s="5" t="s">
         <v>87</v>
@@ -2411,7 +2486,7 @@
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>95</v>
       </c>
@@ -2423,7 +2498,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="5"/>
       <c r="B101" s="5" t="s">
         <v>97</v>
@@ -2436,7 +2511,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
       <c r="B102" s="5" t="s">
         <v>98</v>
@@ -2449,7 +2524,7 @@
         <v>1.2749999999999999E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="5"/>
       <c r="B103" s="5" t="s">
         <v>99</v>
@@ -2462,7 +2537,7 @@
         <v>8.2372000000000003E-5</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="5"/>
       <c r="B104" s="5" t="s">
         <v>101</v>
@@ -2475,872 +2550,875 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="5"/>
       <c r="B105" s="5" t="s">
         <v>102</v>
       </c>
       <c r="C105" s="5"/>
+      <c r="E105" t="s">
+        <v>163</v>
+      </c>
       <c r="H105">
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="5"/>
       <c r="B106" s="5" t="s">
-        <v>103</v>
+        <v>162</v>
       </c>
       <c r="C106" s="5"/>
-      <c r="D106" t="s">
-        <v>104</v>
+      <c r="E106" t="s">
+        <v>164</v>
       </c>
       <c r="H106">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="5"/>
       <c r="B107" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C107" s="5"/>
       <c r="D107" t="s">
+        <v>104</v>
+      </c>
+      <c r="H107">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A108" s="5"/>
+      <c r="B108" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C108" s="5"/>
+      <c r="D108" t="s">
         <v>106</v>
       </c>
-      <c r="H107">
+      <c r="H108">
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A108" s="5" t="s">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B109" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C108" s="5"/>
-      <c r="D108" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H108">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A109" s="5"/>
-      <c r="B109" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="C109" s="5"/>
       <c r="D109" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H109" s="13">
-        <v>3.1415999999999999</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="H109">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="5" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="C110" s="5"/>
       <c r="D110" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H110">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="H110" s="13">
+        <v>3.1415999999999999</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C111" s="5"/>
       <c r="D111" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H111" s="13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="H111">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="5"/>
       <c r="B112" s="5" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C112" s="5"/>
       <c r="D112" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H112" s="14">
-        <v>1.5E-5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H112" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="5"/>
       <c r="B113" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C113" s="5"/>
-      <c r="D113" s="12"/>
-      <c r="H113" s="13">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D113" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H113" s="14">
+        <v>1.5E-5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="5"/>
       <c r="B114" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C114" s="5"/>
       <c r="D114" s="12"/>
       <c r="H114" s="13">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="5"/>
       <c r="B115" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C115" s="5"/>
       <c r="D115" s="12"/>
       <c r="H115" s="13">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C116" s="5"/>
       <c r="D116" s="12"/>
-      <c r="H116" s="14">
-        <v>3.66</v>
-      </c>
-    </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H116" s="13">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="5"/>
       <c r="B117" s="5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C117" s="5"/>
-      <c r="D117" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H117" s="13">
-        <v>0.101325</v>
-      </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D117" s="12"/>
+      <c r="H117" s="14">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="5"/>
       <c r="B118" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C118" s="5"/>
       <c r="D118" s="12" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="H118" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.101325</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="5" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="C119" s="5"/>
-      <c r="H119">
-        <v>0.77905999999999997</v>
-      </c>
-      <c r="I119">
-        <v>0.20709</v>
-      </c>
-      <c r="J119">
-        <v>0</v>
-      </c>
-      <c r="K119">
-        <v>1.3849999999999999E-2</v>
-      </c>
-    </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D119" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H119" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C120" s="5"/>
-      <c r="D120" t="s">
-        <v>90</v>
-      </c>
-      <c r="H120" s="15">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H120">
+        <v>0.77905999999999997</v>
+      </c>
+      <c r="I120">
+        <v>0.20709</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120">
+        <v>1.3849999999999999E-2</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="B121" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C121" s="5"/>
-      <c r="H121">
-        <v>0</v>
-      </c>
-      <c r="I121">
-        <v>0</v>
-      </c>
-      <c r="J121">
-        <v>0</v>
-      </c>
-      <c r="K121">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D121" t="s">
+        <v>90</v>
+      </c>
+      <c r="H121" s="15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="B122" s="5" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="C122" s="5"/>
-      <c r="D122" t="s">
-        <v>50</v>
-      </c>
       <c r="H122">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+      <c r="K122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="B123" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C123" s="5"/>
       <c r="D123" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H123">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="B124" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C124" s="5"/>
       <c r="D124" t="s">
         <v>46</v>
       </c>
       <c r="H124">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="5"/>
+      <c r="B125" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C125" s="5"/>
+      <c r="D125" t="s">
+        <v>46</v>
+      </c>
+      <c r="H125">
         <v>0.6</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A125" s="5" t="s">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B126" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C125" s="5"/>
-      <c r="D125" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H125">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A126" s="5"/>
-      <c r="B126" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="C126" s="5"/>
       <c r="D126" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H126" s="13">
-        <v>3.1415999999999999</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="H126">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="5"/>
       <c r="B127" s="5" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="C127" s="5"/>
       <c r="D127" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H127">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="H127" s="13">
+        <v>3.1415999999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="5"/>
       <c r="B128" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C128" s="5"/>
       <c r="D128" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H128" s="13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="H128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="5"/>
       <c r="B129" s="5" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C129" s="5"/>
       <c r="D129" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H129" s="14">
-        <v>1.5E-5</v>
-      </c>
-    </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H129" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="5"/>
       <c r="B130" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C130" s="5"/>
-      <c r="D130" s="12"/>
-      <c r="H130" s="13">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D130" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H130" s="14">
+        <v>1.5E-5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="5"/>
       <c r="B131" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C131" s="5"/>
       <c r="D131" s="12"/>
       <c r="H131" s="13">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="5"/>
       <c r="B132" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C132" s="5"/>
       <c r="D132" s="12"/>
       <c r="H132" s="13">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="5"/>
       <c r="B133" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C133" s="5"/>
       <c r="D133" s="12"/>
-      <c r="H133" s="14">
-        <v>3.66</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H133" s="13">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="5"/>
       <c r="B134" s="5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C134" s="5"/>
-      <c r="D134" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H134" s="13">
-        <v>0.101325</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D134" s="12"/>
+      <c r="H134" s="14">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="5"/>
       <c r="B135" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C135" s="5"/>
       <c r="D135" s="12" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="H135" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.101325</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="5"/>
       <c r="B136" s="5" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="C136" s="5"/>
-      <c r="H136">
-        <v>0.77905999999999997</v>
-      </c>
-      <c r="I136">
-        <v>0.20709</v>
-      </c>
-      <c r="J136">
-        <v>0</v>
-      </c>
-      <c r="K136">
-        <v>1.3849999999999999E-2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D136" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H136" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="5"/>
       <c r="B137" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C137" s="5"/>
-      <c r="D137" t="s">
-        <v>90</v>
-      </c>
-      <c r="H137" s="15">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H137">
+        <v>0.77905999999999997</v>
+      </c>
+      <c r="I137">
+        <v>0.20709</v>
+      </c>
+      <c r="J137">
+        <v>0</v>
+      </c>
+      <c r="K137">
+        <v>1.3849999999999999E-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="5"/>
       <c r="B138" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C138" s="5"/>
-      <c r="H138">
-        <v>0</v>
-      </c>
-      <c r="I138">
-        <v>0</v>
-      </c>
-      <c r="J138">
-        <v>0</v>
-      </c>
-      <c r="K138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D138" t="s">
+        <v>90</v>
+      </c>
+      <c r="H138" s="15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="5"/>
       <c r="B139" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C139" s="5"/>
+      <c r="H139">
+        <v>0</v>
+      </c>
+      <c r="I139">
+        <v>0</v>
+      </c>
+      <c r="J139">
+        <v>0</v>
+      </c>
+      <c r="K139">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A140" s="5"/>
+      <c r="B140" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C139" s="5"/>
-      <c r="D139" t="s">
+      <c r="C140" s="5"/>
+      <c r="D140" t="s">
         <v>46</v>
       </c>
-      <c r="H139">
+      <c r="H140">
         <v>353</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A140" s="5" t="s">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A141" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B140" s="5" t="s">
+      <c r="B141" s="5" t="s">
         <v>108</v>
-      </c>
-      <c r="C140" s="5"/>
-      <c r="D140" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H140">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A141" s="5"/>
-      <c r="B141" s="5" t="s">
-        <v>113</v>
       </c>
       <c r="C141" s="5"/>
       <c r="D141" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H141" s="13">
-        <v>3.1415999999999999</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="H141">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="5"/>
       <c r="B142" s="5" t="s">
-        <v>37</v>
+        <v>113</v>
       </c>
       <c r="C142" s="5"/>
       <c r="D142" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H142">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="H142" s="13">
+        <v>3.1415999999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="5"/>
       <c r="B143" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C143" s="5"/>
       <c r="D143" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H143" s="13">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="H143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="5"/>
       <c r="B144" s="5" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C144" s="5"/>
       <c r="D144" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H144" s="14">
-        <v>1.5E-5</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H144" s="13">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="5"/>
       <c r="B145" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C145" s="5"/>
-      <c r="D145" s="12"/>
-      <c r="H145" s="13">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D145" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H145" s="14">
+        <v>1.5E-5</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="5"/>
       <c r="B146" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C146" s="5"/>
       <c r="D146" s="12"/>
       <c r="H146" s="13">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="5"/>
       <c r="B147" s="5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C147" s="5"/>
       <c r="D147" s="12"/>
       <c r="H147" s="13">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="5"/>
       <c r="B148" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C148" s="5"/>
       <c r="D148" s="12"/>
-      <c r="H148" s="14">
-        <v>3.66</v>
-      </c>
-    </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H148" s="13">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="5"/>
       <c r="B149" s="5" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C149" s="5"/>
-      <c r="D149" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H149" s="13">
-        <v>0.101325</v>
-      </c>
-    </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D149" s="12"/>
+      <c r="H149" s="14">
+        <v>3.66</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="5"/>
       <c r="B150" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C150" s="5"/>
       <c r="D150" s="12" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="H150" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.101325</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="5"/>
       <c r="B151" s="5" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="C151" s="5"/>
-      <c r="H151">
-        <v>0.77905999999999997</v>
-      </c>
-      <c r="I151">
-        <v>0.20709</v>
-      </c>
-      <c r="J151">
-        <v>0</v>
-      </c>
-      <c r="K151">
-        <v>1.3849999999999999E-2</v>
-      </c>
-    </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D151" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H151" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="5"/>
       <c r="B152" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C152" s="5"/>
-      <c r="D152" t="s">
-        <v>90</v>
-      </c>
-      <c r="H152" s="15">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H152">
+        <v>0.77905999999999997</v>
+      </c>
+      <c r="I152">
+        <v>0.20709</v>
+      </c>
+      <c r="J152">
+        <v>0</v>
+      </c>
+      <c r="K152">
+        <v>1.3849999999999999E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="5"/>
       <c r="B153" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C153" s="5"/>
-      <c r="H153">
-        <v>0</v>
-      </c>
-      <c r="I153">
-        <v>0</v>
-      </c>
-      <c r="J153">
-        <v>0</v>
-      </c>
-      <c r="K153">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D153" t="s">
+        <v>90</v>
+      </c>
+      <c r="H153" s="15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="5"/>
       <c r="B154" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C154" s="5"/>
+      <c r="H154">
+        <v>0</v>
+      </c>
+      <c r="I154">
+        <v>0</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+      <c r="K154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A155" s="5"/>
+      <c r="B155" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C154" s="5"/>
-      <c r="D154" t="s">
+      <c r="C155" s="5"/>
+      <c r="D155" t="s">
         <v>46</v>
       </c>
-      <c r="H154">
+      <c r="H155">
         <v>353</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A155" s="5" t="s">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A156" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B155" s="5" t="s">
+      <c r="B156" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C155" s="5"/>
-      <c r="D155" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H155" s="13">
-        <v>0.101325</v>
-      </c>
-    </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A156" s="5"/>
-      <c r="B156" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="C156" s="5"/>
       <c r="D156" s="12" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="H156" s="13">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+        <v>0.101325</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="5"/>
       <c r="B157" s="5" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="C157" s="5"/>
-      <c r="H157">
-        <v>0.77905999999999997</v>
-      </c>
-      <c r="I157">
-        <v>0.20709</v>
-      </c>
-      <c r="J157">
-        <v>0</v>
-      </c>
-      <c r="K157">
-        <v>1.3849999999999999E-2</v>
-      </c>
-    </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D157" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="H157" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="5"/>
       <c r="B158" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C158" s="5"/>
+      <c r="H158">
+        <v>0.77905999999999997</v>
+      </c>
+      <c r="I158">
+        <v>0.20709</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+      <c r="K158">
+        <v>1.3849999999999999E-2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A159" s="5"/>
+      <c r="B159" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C158" s="5"/>
-      <c r="D158" s="12" t="s">
+      <c r="C159" s="5"/>
+      <c r="D159" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="H158" s="13">
+      <c r="H159" s="13">
         <v>3.1415999999999999</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A159" s="5" t="s">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A160" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B159" s="5" t="s">
+      <c r="B160" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C159" s="5"/>
-      <c r="H159">
+      <c r="C160" s="5"/>
+      <c r="H160">
         <v>2</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A160" s="5"/>
-      <c r="B160" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="C160" s="5"/>
-      <c r="D160" t="s">
-        <v>50</v>
-      </c>
-      <c r="H160">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="5"/>
       <c r="B161" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C161" s="5"/>
       <c r="D161" t="s">
-        <v>121</v>
+        <v>50</v>
       </c>
       <c r="H161">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="5"/>
       <c r="B162" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C162" s="5"/>
-      <c r="D162" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="H162" s="13">
-        <v>0.101325</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D162" t="s">
+        <v>121</v>
+      </c>
+      <c r="H162">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="5"/>
       <c r="B163" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C163" s="5"/>
-      <c r="D163" t="s">
-        <v>46</v>
-      </c>
-      <c r="H163">
-        <v>288.14999999999998</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D163" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H163" s="13">
+        <v>0.101325</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="5"/>
       <c r="B164" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C164" s="5"/>
+      <c r="D164" t="s">
+        <v>46</v>
+      </c>
       <c r="H164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.3">
+        <v>288.14999999999998</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="5"/>
       <c r="B165" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C165" s="5"/>
       <c r="H165">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="5"/>
       <c r="B166" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C166" s="5"/>
       <c r="H166">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="5"/>
       <c r="B167" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C167" s="5"/>
       <c r="H167">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="5"/>
       <c r="B168" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C168" s="5"/>
       <c r="H168">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="5"/>
       <c r="B169" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C169" s="5"/>
       <c r="H169">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="5"/>
       <c r="B170" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C170" s="5"/>
-      <c r="D170" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H170" s="13">
-        <v>3.1415999999999999</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H170">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="5"/>
       <c r="B171" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C171" s="5"/>
       <c r="D171" s="12" t="s">
@@ -3350,57 +3428,286 @@
         <v>3.1415999999999999</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="5"/>
       <c r="B172" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C172" s="5"/>
-      <c r="D172" t="s">
-        <v>133</v>
-      </c>
-      <c r="H172" s="15">
-        <v>5.0000000000000002E-5</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D172" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H172" s="13">
+        <v>3.1415999999999999</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="5"/>
       <c r="B173" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C173" s="5"/>
       <c r="D173" t="s">
+        <v>133</v>
+      </c>
+      <c r="H173" s="15">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A174" s="5"/>
+      <c r="B174" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C174" s="5"/>
+      <c r="D174" t="s">
         <v>135</v>
       </c>
-      <c r="H173">
+      <c r="H174">
         <f>0.00001*10</f>
         <v>1E-4</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A174" s="5"/>
-      <c r="B174" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C174" s="5"/>
-      <c r="D174" t="s">
-        <v>137</v>
-      </c>
-      <c r="H174">
-        <v>1.7999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="5"/>
       <c r="B175" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C175" s="5"/>
       <c r="D175" t="s">
+        <v>137</v>
+      </c>
+      <c r="H175">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A176" s="5"/>
+      <c r="B176" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C176" s="5"/>
+      <c r="D176" t="s">
         <v>75</v>
       </c>
-      <c r="H175">
+      <c r="H176">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A177" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B177" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C177" s="5"/>
+      <c r="D177" t="s">
+        <v>75</v>
+      </c>
+      <c r="H177">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A178" s="8"/>
+      <c r="B178" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="D178" t="s">
+        <v>65</v>
+      </c>
+      <c r="H178">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A179" s="8"/>
+      <c r="B179" s="5"/>
+      <c r="C179" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D179" t="s">
+        <v>75</v>
+      </c>
+      <c r="H179">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A180" s="8"/>
+      <c r="B180" s="5"/>
+      <c r="C180" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="D180" t="s">
+        <v>145</v>
+      </c>
+      <c r="H180">
+        <v>1.0000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A181" s="8"/>
+      <c r="B181" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C181" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D181" t="s">
+        <v>146</v>
+      </c>
+      <c r="H181" s="15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="K181" s="15"/>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A182" s="8"/>
+      <c r="B182" s="5"/>
+      <c r="C182" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D182" t="s">
+        <v>75</v>
+      </c>
+      <c r="H182" s="15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A183" s="8"/>
+      <c r="B183" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="C183" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D183" t="s">
+        <v>148</v>
+      </c>
+      <c r="H183" s="15">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A184" s="8"/>
+      <c r="B184" s="5"/>
+      <c r="C184" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D184" t="s">
+        <v>75</v>
+      </c>
+      <c r="H184">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A185" s="8"/>
+      <c r="B185" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="C185" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D185" t="s">
+        <v>148</v>
+      </c>
+      <c r="H185">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A186" s="8"/>
+      <c r="B186" s="5"/>
+      <c r="C186" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D186" t="s">
+        <v>75</v>
+      </c>
+      <c r="H186" s="15">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A187" s="8"/>
+      <c r="B187" s="5"/>
+      <c r="C187" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D187" t="s">
+        <v>145</v>
+      </c>
+      <c r="H187" s="15">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A188" s="8"/>
+      <c r="B188" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C188" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="H188" s="15">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A189" s="8"/>
+      <c r="B189" s="5"/>
+      <c r="C189" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H189" s="15">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A190" s="8"/>
+      <c r="B190" s="5"/>
+      <c r="C190" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A191" s="8"/>
+      <c r="B191" s="5"/>
+      <c r="C191" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="H191" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A192" s="8"/>
+      <c r="B192" s="5"/>
+      <c r="C192" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="H192" s="15">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A193" s="8"/>
+      <c r="B193" s="5"/>
+      <c r="C193" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H193" s="15">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>